<commit_message>
Updated my hours log
</commit_message>
<xml_diff>
--- a/Sprint 2 Hours Log -- Mason.xlsx
+++ b/Sprint 2 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -48,15 +48,41 @@
   </si>
   <si>
     <t>I added the action listener and menu item to the gameboard class and added a resetQueue method to the TileQueue class</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Added colors just for the fun of it</t>
+  </si>
+  <si>
+    <t>Added the menu, menu item, and empty action listener for the Top 10 List</t>
+  </si>
+  <si>
+    <t>SF-15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -120,18 +146,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -454,7 +486,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -494,16 +526,32 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="A3" s="2">
+        <v>42829</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="A4" s="2">
+        <v>42829</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>

</xml_diff>

<commit_message>
Made some UI changes to how the queue looks. I think this looks better than the way I had it before when I changed the colors and the tiles were huge.
</commit_message>
<xml_diff>
--- a/Sprint 2 Hours Log -- Mason.xlsx
+++ b/Sprint 2 Hours Log -- Mason.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -60,15 +60,31 @@
   </si>
   <si>
     <t>SF-15</t>
+  </si>
+  <si>
+    <t>preGameScreen takes the name and places it into the GameBoard as playerName</t>
+  </si>
+  <si>
+    <t>SF-2</t>
+  </si>
+  <si>
+    <t>preGameScreen gives the option of a timed game or untimed game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -146,18 +162,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -486,7 +505,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -554,16 +573,32 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="A5" s="2">
+        <v>42830</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="A6" s="2">
+        <v>42830</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Added a checkWin method for the gameboard class and refactored some existing code for stopping the game if you won. This should set us up to be able to store the names and scores for the top ten
</commit_message>
<xml_diff>
--- a/Sprint 2 Hours Log -- Mason.xlsx
+++ b/Sprint 2 Hours Log -- Mason.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -69,15 +69,25 @@
   </si>
   <si>
     <t>preGameScreen gives the option of a timed game or untimed game</t>
+  </si>
+  <si>
+    <t>Added a checkWin method and refactored some of the existing code for stopping when the game is won</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -162,18 +172,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -505,7 +518,7 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -601,10 +614,18 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="A7" s="2">
+        <v>42840</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>

</xml_diff>